<commit_message>
arreglos al ingreso de archivos
</commit_message>
<xml_diff>
--- a/public/uploads/Equipos y Camionetas prueba.xlsx
+++ b/public/uploads/Equipos y Camionetas prueba.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabri\Desktop\archivos qu eno puedo ingresar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{735FDF72-2909-4808-8664-C76FB6631F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9128454F-870A-4E98-A08A-388AEBCE280E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
   <si>
     <t>CONTRATO</t>
   </si>
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>KILOMETRAJE ACTUAL</t>
-  </si>
-  <si>
-    <t>asdasdse</t>
   </si>
 </sst>
 </file>
@@ -316,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -357,32 +354,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="hair">
         <color indexed="64"/>
       </top>
@@ -448,30 +419,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -538,32 +485,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -582,134 +503,110 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1012,10 +909,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,100 +925,125 @@
     <col min="9" max="13" width="11.42578125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="41.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:13" ht="41.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="L1" s="32" t="s">
+      <c r="L1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="M1" s="32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="37"/>
+    <row r="2" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4600020368</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="10">
+        <v>44834</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="14">
+        <v>108017</v>
+      </c>
+      <c r="J2" s="16">
+        <v>101651</v>
+      </c>
+      <c r="K2" s="17">
+        <f>+J2-I2</f>
+        <v>-6366</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="22">
+        <v>44869</v>
+      </c>
     </row>
     <row r="3" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="10">
-        <v>44834</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="14">
-        <v>108017</v>
-      </c>
-      <c r="J3" s="16">
-        <v>101651</v>
-      </c>
-      <c r="K3" s="17">
-        <f>+J3-I3</f>
-        <v>-6366</v>
-      </c>
-      <c r="L3" s="18" t="s">
+      <c r="F3" s="11">
+        <v>44684</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="4"/>
+      <c r="I3" s="15">
+        <v>20000</v>
+      </c>
+      <c r="J3" s="19">
+        <v>15321</v>
+      </c>
+      <c r="K3" s="20">
+        <f t="shared" ref="K3:K21" si="0">+J3-I3</f>
+        <v>-4679</v>
+      </c>
+      <c r="L3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M3" s="19" t="s">
-        <v>58</v>
+      <c r="M3" s="22">
+        <v>44869</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
@@ -1132,35 +1054,35 @@
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="11">
-        <v>44684</v>
+        <v>44600</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>45</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="15">
-        <v>20000</v>
-      </c>
-      <c r="J4" s="20">
-        <v>15321</v>
-      </c>
-      <c r="K4" s="21">
-        <f t="shared" ref="K4:K22" si="0">+J4-I4</f>
-        <v>-4679</v>
-      </c>
-      <c r="L4" s="22" t="s">
+        <v>25000</v>
+      </c>
+      <c r="J4" s="19">
+        <v>23125</v>
+      </c>
+      <c r="K4" s="20">
+        <f t="shared" si="0"/>
+        <v>-1875</v>
+      </c>
+      <c r="L4" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="22">
         <v>44869</v>
       </c>
     </row>
@@ -1172,7 +1094,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>11</v>
@@ -1181,26 +1103,26 @@
         <v>8</v>
       </c>
       <c r="F5" s="11">
-        <v>44600</v>
+        <v>44615</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>45</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="15">
-        <v>25000</v>
-      </c>
-      <c r="J5" s="20">
-        <v>23125</v>
-      </c>
-      <c r="K5" s="21">
+        <v>20000</v>
+      </c>
+      <c r="J5" s="19">
+        <v>15181</v>
+      </c>
+      <c r="K5" s="20">
         <f t="shared" si="0"/>
-        <v>-1875</v>
-      </c>
-      <c r="L5" s="22" t="s">
+        <v>-4819</v>
+      </c>
+      <c r="L5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M5" s="22">
         <v>44869</v>
       </c>
     </row>
@@ -1212,39 +1134,39 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="11">
-        <v>44615</v>
+        <v>44831</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="15">
-        <v>20000</v>
-      </c>
-      <c r="J6" s="20">
-        <v>15181</v>
-      </c>
-      <c r="K6" s="21">
+        <v>30583</v>
+      </c>
+      <c r="J6" s="19">
+        <v>22943</v>
+      </c>
+      <c r="K6" s="20">
         <f t="shared" si="0"/>
-        <v>-4819</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="M6" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+        <v>-7640</v>
+      </c>
+      <c r="L6" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4600020368</v>
       </c>
@@ -1252,39 +1174,35 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="11">
-        <v>44831</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>46</v>
-      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="13"/>
       <c r="H7" s="4"/>
       <c r="I7" s="15">
-        <v>30583</v>
-      </c>
-      <c r="J7" s="20">
-        <v>22943</v>
-      </c>
-      <c r="K7" s="21">
+        <v>10000</v>
+      </c>
+      <c r="J7" s="19">
+        <v>7120</v>
+      </c>
+      <c r="K7" s="20">
         <f t="shared" si="0"/>
-        <v>-7640</v>
-      </c>
-      <c r="L7" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <v>-2880</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4600020368</v>
       </c>
@@ -1292,7 +1210,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>7</v>
@@ -1300,27 +1218,31 @@
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="11">
+        <v>44789</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>45</v>
+      </c>
       <c r="H8" s="4"/>
       <c r="I8" s="15">
-        <v>10000</v>
-      </c>
-      <c r="J8" s="20">
-        <v>7120</v>
-      </c>
-      <c r="K8" s="21">
-        <f t="shared" si="0"/>
-        <v>-2880</v>
-      </c>
-      <c r="L8" s="22" t="s">
+        <v>20000</v>
+      </c>
+      <c r="J8" s="19">
+        <v>13438</v>
+      </c>
+      <c r="K8" s="20">
+        <f>+J8-I8</f>
+        <v>-6562</v>
+      </c>
+      <c r="L8" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="M8" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4600020368</v>
       </c>
@@ -1328,7 +1250,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>7</v>
@@ -1336,31 +1258,27 @@
       <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="11">
-        <v>44789</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>45</v>
-      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="13"/>
       <c r="H9" s="4"/>
       <c r="I9" s="15">
-        <v>20000</v>
-      </c>
-      <c r="J9" s="20">
-        <v>13438</v>
-      </c>
-      <c r="K9" s="21">
-        <f>+J9-I9</f>
-        <v>-6562</v>
-      </c>
-      <c r="L9" s="22" t="s">
+        <v>10000</v>
+      </c>
+      <c r="J9" s="19">
+        <v>6130</v>
+      </c>
+      <c r="K9" s="20">
+        <f t="shared" si="0"/>
+        <v>-3870</v>
+      </c>
+      <c r="L9" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M9" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4600020368</v>
       </c>
@@ -1368,7 +1286,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>7</v>
@@ -1376,27 +1294,31 @@
       <c r="E10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="11">
+        <v>44603</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>48</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="15">
-        <v>10000</v>
-      </c>
-      <c r="J10" s="20">
-        <v>6130</v>
-      </c>
-      <c r="K10" s="21">
+        <v>20100</v>
+      </c>
+      <c r="J10" s="19">
+        <v>18390</v>
+      </c>
+      <c r="K10" s="20">
         <f t="shared" si="0"/>
-        <v>-3870</v>
-      </c>
-      <c r="L10" s="22" t="s">
+        <v>-1710</v>
+      </c>
+      <c r="L10" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="M10" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>4600020368</v>
       </c>
@@ -1404,35 +1326,31 @@
         <v>5</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="11">
-        <v>44603</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>48</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="4"/>
       <c r="I11" s="15">
-        <v>20100</v>
-      </c>
-      <c r="J11" s="20">
-        <v>18390</v>
-      </c>
-      <c r="K11" s="21">
+        <v>10000</v>
+      </c>
+      <c r="J11" s="19">
+        <v>7575</v>
+      </c>
+      <c r="K11" s="20">
         <f t="shared" si="0"/>
-        <v>-1710</v>
-      </c>
-      <c r="L11" s="22" t="s">
+        <v>-2425</v>
+      </c>
+      <c r="L11" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M11" s="23">
+      <c r="M11" s="22">
         <v>44869</v>
       </c>
     </row>
@@ -1444,13 +1362,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F12" s="11"/>
       <c r="G12" s="13"/>
@@ -1458,17 +1376,17 @@
       <c r="I12" s="15">
         <v>10000</v>
       </c>
-      <c r="J12" s="20">
-        <v>7575</v>
-      </c>
-      <c r="K12" s="21">
+      <c r="J12" s="19">
+        <v>5691</v>
+      </c>
+      <c r="K12" s="20">
         <f t="shared" si="0"/>
-        <v>-2425</v>
-      </c>
-      <c r="L12" s="22" t="s">
+        <v>-4309</v>
+      </c>
+      <c r="L12" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="22">
         <v>44869</v>
       </c>
     </row>
@@ -1476,15 +1394,13 @@
       <c r="A13" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>5</v>
+      <c r="B13" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>7</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D13" s="9"/>
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1494,17 +1410,17 @@
       <c r="I13" s="15">
         <v>10000</v>
       </c>
-      <c r="J13" s="20">
-        <v>5691</v>
-      </c>
-      <c r="K13" s="21">
+      <c r="J13" s="19">
+        <v>6855</v>
+      </c>
+      <c r="K13" s="20">
         <f t="shared" si="0"/>
-        <v>-4309</v>
-      </c>
-      <c r="L13" s="22" t="s">
+        <v>-3145</v>
+      </c>
+      <c r="L13" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="22">
         <v>44869</v>
       </c>
     </row>
@@ -1512,45 +1428,45 @@
       <c r="A14" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>22</v>
+      <c r="B14" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="13"/>
       <c r="H14" s="4"/>
       <c r="I14" s="15">
-        <v>10000</v>
-      </c>
-      <c r="J14" s="20">
-        <v>6855</v>
-      </c>
-      <c r="K14" s="21">
+        <v>887</v>
+      </c>
+      <c r="J14" s="19">
+        <v>712.4</v>
+      </c>
+      <c r="K14" s="24">
         <f t="shared" si="0"/>
-        <v>-3145</v>
-      </c>
-      <c r="L14" s="22" t="s">
+        <v>-174.60000000000002</v>
+      </c>
+      <c r="L14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M14" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B15" s="29" t="s">
-        <v>24</v>
+      <c r="B15" s="28" t="s">
+        <v>27</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="2" t="s">
@@ -1560,125 +1476,129 @@
       <c r="G15" s="13"/>
       <c r="H15" s="4"/>
       <c r="I15" s="15">
-        <v>887</v>
-      </c>
-      <c r="J15" s="20">
-        <v>712.4</v>
-      </c>
-      <c r="K15" s="25">
+        <v>1000</v>
+      </c>
+      <c r="J15" s="25">
+        <v>915</v>
+      </c>
+      <c r="K15" s="24">
         <f t="shared" si="0"/>
-        <v>-174.60000000000002</v>
-      </c>
-      <c r="L15" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="M15" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+        <v>-85</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="M15" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="13"/>
+      <c r="F16" s="11">
+        <v>44842</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>50</v>
+      </c>
       <c r="H16" s="4"/>
       <c r="I16" s="15">
-        <v>1000</v>
-      </c>
-      <c r="J16" s="26">
-        <v>915</v>
-      </c>
-      <c r="K16" s="25">
+        <v>1255</v>
+      </c>
+      <c r="J16" s="19">
+        <v>1033</v>
+      </c>
+      <c r="K16" s="24">
         <f t="shared" si="0"/>
-        <v>-85</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="M16" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+        <v>-222</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="11">
-        <v>44842</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>50</v>
-      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="4"/>
       <c r="I17" s="15">
-        <v>1255</v>
-      </c>
-      <c r="J17" s="20">
-        <v>1033</v>
-      </c>
-      <c r="K17" s="25">
+        <v>250</v>
+      </c>
+      <c r="J17" s="19">
+        <v>135.19999999999999</v>
+      </c>
+      <c r="K17" s="24">
         <f t="shared" si="0"/>
-        <v>-222</v>
+        <v>-114.80000000000001</v>
       </c>
       <c r="L17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="M17" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>27</v>
+      <c r="B18" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="13"/>
+      <c r="F18" s="11">
+        <v>44732</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>51</v>
+      </c>
       <c r="H18" s="4"/>
       <c r="I18" s="15">
-        <v>250</v>
-      </c>
-      <c r="J18" s="20">
-        <v>135.19999999999999</v>
-      </c>
-      <c r="K18" s="25">
+        <v>700</v>
+      </c>
+      <c r="J18" s="19">
+        <v>608.1</v>
+      </c>
+      <c r="K18" s="24">
         <f t="shared" si="0"/>
-        <v>-114.80000000000001</v>
+        <v>-91.899999999999977</v>
       </c>
       <c r="L18" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M18" s="22">
         <v>44869</v>
       </c>
     </row>
@@ -1686,37 +1606,37 @@
       <c r="A19" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="11">
-        <v>44732</v>
+        <v>44713</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="15">
-        <v>700</v>
-      </c>
-      <c r="J19" s="20">
-        <v>608.1</v>
-      </c>
-      <c r="K19" s="25">
+        <v>523</v>
+      </c>
+      <c r="J19" s="19">
+        <v>508.9</v>
+      </c>
+      <c r="K19" s="24">
         <f t="shared" si="0"/>
-        <v>-91.899999999999977</v>
-      </c>
-      <c r="L19" s="13" t="s">
+        <v>-14.100000000000023</v>
+      </c>
+      <c r="L19" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M19" s="23">
+      <c r="M19" s="22">
         <v>44869</v>
       </c>
     </row>
@@ -1724,75 +1644,71 @@
       <c r="A20" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>31</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="11">
-        <v>44713</v>
+        <v>44725</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="15">
-        <v>523</v>
-      </c>
-      <c r="J20" s="20">
-        <v>508.9</v>
-      </c>
-      <c r="K20" s="25">
+        <v>876</v>
+      </c>
+      <c r="J20" s="19">
+        <v>909.4</v>
+      </c>
+      <c r="K20" s="24">
         <f t="shared" si="0"/>
-        <v>-14.100000000000023</v>
-      </c>
-      <c r="L20" s="22" t="s">
+        <v>33.399999999999977</v>
+      </c>
+      <c r="L20" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="M20" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="M20" s="22">
+        <v>44869</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B21" s="29" t="s">
-        <v>31</v>
+      <c r="B21" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="11">
-        <v>44725</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>53</v>
-      </c>
+      <c r="F21" s="11"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="4"/>
       <c r="I21" s="15">
-        <v>876</v>
-      </c>
-      <c r="J21" s="20">
-        <v>909.4</v>
-      </c>
-      <c r="K21" s="25">
+        <v>650</v>
+      </c>
+      <c r="J21" s="19">
+        <v>494.9</v>
+      </c>
+      <c r="K21" s="24">
         <f t="shared" si="0"/>
-        <v>33.399999999999977</v>
-      </c>
-      <c r="L21" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="M21" s="23">
+        <v>-155.10000000000002</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="M21" s="22">
         <v>44869</v>
       </c>
     </row>
@@ -1800,94 +1716,45 @@
       <c r="A22" s="1">
         <v>4600020368</v>
       </c>
-      <c r="B22" s="29" t="s">
-        <v>24</v>
+      <c r="B22" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="E22" s="2" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="F22" s="11"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="4"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="15">
-        <v>650</v>
-      </c>
-      <c r="J22" s="20">
-        <v>494.9</v>
-      </c>
-      <c r="K22" s="25">
-        <f t="shared" si="0"/>
-        <v>-155.10000000000002</v>
-      </c>
-      <c r="L22" s="24" t="s">
+        <v>10000</v>
+      </c>
+      <c r="J22" s="25">
+        <v>9618</v>
+      </c>
+      <c r="K22" s="20">
+        <f>+J22-I22</f>
+        <v>-382</v>
+      </c>
+      <c r="L22" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="M22" s="23">
-        <v>44869</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>4600020368</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="15">
-        <v>10000</v>
-      </c>
-      <c r="J23" s="26">
-        <v>9618</v>
-      </c>
-      <c r="K23" s="21">
-        <f>+J23-I23</f>
-        <v>-382</v>
-      </c>
-      <c r="L23" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="M23" s="27" t="s">
+      <c r="M22" s="26" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-  </mergeCells>
-  <conditionalFormatting sqref="K3:K22">
+  <conditionalFormatting sqref="K2:K21">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
+  <conditionalFormatting sqref="K22">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>

</xml_diff>